<commit_message>
code to save discounts and manipulation in invoice
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -1,38 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Documents\workspace-spring-tool-suite-4-4.17.1.RELEASE\POSProject_ZainAleem\pos_backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Inventory Management\pos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9EFE27-8F13-4407-BDA4-0F698C2B40D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice Template" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>BILL TO</t>
   </si>
@@ -68,16 +56,19 @@
   </si>
   <si>
     <t>${OperatorName}</t>
+  </si>
+  <si>
+    <t>TRADE PRICE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -204,8 +195,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="31">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -237,23 +228,22 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -265,7 +255,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -287,7 +277,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -308,6 +298,105 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2590799</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>915077</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB85E6F3-3FCB-405B-BBF6-F34CF3083179}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2876549" y="200024"/>
+          <a:ext cx="5268003" cy="895351"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1466850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2520635</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D68AD1B-FB19-4890-8517-06EBA065A8CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1752600" y="228600"/>
+          <a:ext cx="1053785" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -606,152 +695,165 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF8496B0"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="52.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="5" width="20.28515625" customWidth="1"/>
+    <col min="4" max="6" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A1" s="26"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="29"/>
-    </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+    <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28"/>
+    </row>
+    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="20"/>
-    </row>
-    <row r="3" spans="1:5" ht="30.75" customHeight="1">
+      <c r="E2" s="3"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="23"/>
-    </row>
-    <row r="4" spans="1:5" s="12" customFormat="1" ht="18.75" customHeight="1">
+      <c r="E3" s="4"/>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="23"/>
-    </row>
-    <row r="5" spans="1:5" s="12" customFormat="1" ht="18.75" customHeight="1">
+      <c r="E4" s="4"/>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="23"/>
-    </row>
-    <row r="6" spans="1:5" s="12" customFormat="1" ht="18.75" customHeight="1">
+      <c r="E5" s="4"/>
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="10"/>
       <c r="C6" s="1"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1">
+      <c r="E6" s="4"/>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="1"/>
+      <c r="F7" s="23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1">
+    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="1"/>
+      <c r="F8" s="24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1">
+    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="22"/>
-    </row>
-    <row r="10" spans="1:5" ht="16.5" customHeight="1">
+      <c r="E9" s="1"/>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="C10" s="7"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="21"/>
-    </row>
-    <row r="11" spans="1:5" s="12" customFormat="1" ht="18" customHeight="1">
+      <c r="E10" s="1"/>
+      <c r="F10" s="20"/>
+    </row>
+    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="10"/>
       <c r="C11" s="9"/>
-      <c r="E11" s="22"/>
-    </row>
-    <row r="12" spans="1:5" ht="18" customHeight="1">
-      <c r="A12" s="26"/>
-      <c r="B12" s="30" t="s">
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="25"/>
+      <c r="B12" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18" customHeight="1">
+    <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-    </row>
-    <row r="14" spans="1:5" ht="19.5" customHeight="1">
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="15"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="11"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-    </row>
-    <row r="21" spans="3:3" ht="15" customHeight="1">
-      <c r="C21" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modification in invoice template
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Inventory Management\pos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9EFE27-8F13-4407-BDA4-0F698C2B40D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFA5BB1-C9B3-4B7F-AB54-96E27FE6103D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,9 +31,6 @@
     <t>QTY</t>
   </si>
   <si>
-    <t>UNIT PRICE</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -59,6 +56,9 @@
   </si>
   <si>
     <t>TRADE PRICE</t>
+  </si>
+  <si>
+    <t>RETAIL PRICE</t>
   </si>
 </sst>
 </file>
@@ -388,6 +388,50 @@
         <a:xfrm>
           <a:off x="1752600" y="228600"/>
           <a:ext cx="1053785" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>15363</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>162540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1305847</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>25518</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5389CE45-011A-40B1-174B-F725F19AEA56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15363" y="5524193"/>
+          <a:ext cx="8526411" cy="2259591"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -703,8 +747,8 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -734,7 +778,7 @@
     <row r="3" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="4"/>
@@ -744,7 +788,7 @@
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="4"/>
@@ -754,7 +798,7 @@
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="4"/>
@@ -778,25 +822,25 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
@@ -825,13 +869,13 @@
         <v>2</v>
       </c>
       <c r="D12" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="30" t="s">
         <v>3</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>